<commit_message>
corrected options. -> defaultptn has to be FALSE
</commit_message>
<xml_diff>
--- a/perf.xlsx
+++ b/perf.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Research\project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48A4184-FCAE-44E2-8AF9-FA0BE3883A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA0983E-AFFB-4A3D-B968-E79C2D71C3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14580" yWindow="1160" windowWidth="22680" windowHeight="15370" xr2:uid="{71B9B3C5-B210-445B-8D29-E805313DDE71}"/>
+    <workbookView xWindow="11560" yWindow="3570" windowWidth="24050" windowHeight="15370" activeTab="1" xr2:uid="{71B9B3C5-B210-445B-8D29-E805313DDE71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="quandles" sheetId="4" r:id="rId2"/>
+    <sheet name="semigroups" sheetId="3" r:id="rId3"/>
+    <sheet name="quasigroups" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
   <si>
     <t>Semigroups</t>
   </si>
@@ -87,6 +90,39 @@
   </si>
   <si>
     <t>Experiments done on musca</t>
+  </si>
+  <si>
+    <t>Quandles</t>
+  </si>
+  <si>
+    <t>#models/sec</t>
+  </si>
+  <si>
+    <t>nauty outputs</t>
+  </si>
+  <si>
+    <t>A181769</t>
+  </si>
+  <si>
+    <t>nauty Wall clock time (s)</t>
+  </si>
+  <si>
+    <t>nauty cpu time (s)</t>
+  </si>
+  <si>
+    <t>loops</t>
+  </si>
+  <si>
+    <t>mlex cpu time (s)</t>
+  </si>
+  <si>
+    <t>#nauty outputs</t>
+  </si>
+  <si>
+    <t>(latin square formulation)</t>
+  </si>
+  <si>
+    <t>3 operations</t>
   </si>
 </sst>
 </file>
@@ -441,36 +477,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{070350DB-BF20-4F0F-BCA3-734AB117EDB9}">
-  <dimension ref="A3:M33"/>
+  <dimension ref="A3:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -478,219 +514,916 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10">
         <v>15973</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>28634</v>
       </c>
       <c r="E10">
+        <v>5628898</v>
+      </c>
+      <c r="F10">
         <f>5+4/60</f>
         <v>5.0666666666666664</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>17.95</v>
       </c>
       <c r="J10">
+        <f>E10/304</f>
+        <v>18516.111842105263</v>
+      </c>
+      <c r="K10">
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>9</v>
       </c>
       <c r="B16">
         <v>11</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>11</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>25538</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>4</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>10</v>
       </c>
       <c r="B17">
         <v>18</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>18</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>230984</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>32</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <f>18*60+38</f>
         <v>1118</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>49</v>
+      </c>
+      <c r="D21">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22">
         <v>12</v>
       </c>
-      <c r="B21">
+      <c r="C22">
         <v>2684</v>
       </c>
-      <c r="D21">
+      <c r="D22">
+        <v>2684</v>
+      </c>
+      <c r="E22">
         <v>193368</v>
       </c>
-      <c r="E21">
+      <c r="F22">
         <v>369</v>
       </c>
-      <c r="F21">
+      <c r="G22">
         <f>9*60+45</f>
         <v>585</v>
       </c>
-      <c r="I21">
+      <c r="J22">
         <v>10605</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29">
         <v>7</v>
       </c>
-      <c r="B28">
+      <c r="C29">
         <v>12147</v>
       </c>
-      <c r="C28">
+      <c r="D29">
         <v>23746</v>
       </c>
-      <c r="D28">
+      <c r="E29">
         <v>223808</v>
       </c>
-      <c r="E28">
+      <c r="F29">
         <v>145</v>
       </c>
-      <c r="F28">
+      <c r="G29">
         <v>71</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N29" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="M30">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="J31" t="s">
+        <v>18</v>
+      </c>
+      <c r="N31">
         <f>12147*2-23746</f>
         <v>548</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>14</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H32" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <v>16</v>
+      </c>
+      <c r="C33">
+        <v>16</v>
+      </c>
+      <c r="E33">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35">
         <v>6</v>
       </c>
-      <c r="B32">
+      <c r="B35">
         <v>208</v>
       </c>
-      <c r="D32">
+      <c r="C35">
+        <v>208</v>
+      </c>
+      <c r="E35">
         <v>41069</v>
       </c>
-      <c r="E32">
+      <c r="F35">
         <v>4</v>
       </c>
-      <c r="G32">
+      <c r="H35">
         <v>1800</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36">
         <v>7</v>
       </c>
-      <c r="B33">
+      <c r="B36">
         <v>911</v>
       </c>
-      <c r="D33">
+      <c r="C36">
+        <v>911</v>
+      </c>
+      <c r="E36">
         <v>968795</v>
       </c>
-      <c r="E33">
+      <c r="F36">
         <v>93</v>
+      </c>
+      <c r="J36">
+        <f>E36/93</f>
+        <v>10417.150537634408</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <v>20</v>
+      </c>
+      <c r="D39">
+        <v>22</v>
+      </c>
+      <c r="E39">
+        <v>190</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>6</v>
+      </c>
+      <c r="C40">
+        <v>72</v>
+      </c>
+      <c r="D40">
+        <v>73</v>
+      </c>
+      <c r="E40">
+        <v>1833</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <f>E41/13</f>
+        <v>1700.3076923076924</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="C41">
+        <v>293</v>
+      </c>
+      <c r="D41">
+        <v>298</v>
+      </c>
+      <c r="E41">
+        <v>22104</v>
+      </c>
+      <c r="F41">
+        <v>13</v>
+      </c>
+      <c r="J41">
+        <f>E42/F42</f>
+        <v>1187.6534653465346</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>1572</v>
+      </c>
+      <c r="D42">
+        <v>1581</v>
+      </c>
+      <c r="E42">
+        <v>359859</v>
+      </c>
+      <c r="F42">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1C48C7-82EF-4B8E-B79C-E1931327BF0A}">
+  <dimension ref="A4:K14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>190</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>72</v>
+      </c>
+      <c r="D7">
+        <v>73</v>
+      </c>
+      <c r="E7">
+        <v>1833</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>293</v>
+      </c>
+      <c r="D8">
+        <v>298</v>
+      </c>
+      <c r="E8">
+        <v>22104</v>
+      </c>
+      <c r="G8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>1572</v>
+      </c>
+      <c r="D9">
+        <v>1581</v>
+      </c>
+      <c r="E9">
+        <v>359859</v>
+      </c>
+      <c r="G9">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>11079</v>
+      </c>
+      <c r="E10">
+        <v>7691008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54125112-47BB-49F9-B19F-D459CC1D822A}">
+  <dimension ref="A4:K7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1160</v>
+      </c>
+      <c r="C5">
+        <v>1160</v>
+      </c>
+      <c r="D5">
+        <v>1915</v>
+      </c>
+      <c r="E5">
+        <v>90536</v>
+      </c>
+      <c r="F5">
+        <v>4.11374</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>10.243</v>
+      </c>
+      <c r="K5">
+        <f>E5/F5</f>
+        <v>22008.196920563769</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>15973</v>
+      </c>
+      <c r="C6">
+        <v>15973</v>
+      </c>
+      <c r="D6">
+        <v>28634</v>
+      </c>
+      <c r="E6">
+        <v>5628898</v>
+      </c>
+      <c r="F6">
+        <v>329.16300000000001</v>
+      </c>
+      <c r="G6">
+        <v>339</v>
+      </c>
+      <c r="H6">
+        <v>1011.241</v>
+      </c>
+      <c r="K6">
+        <f>E6/F6</f>
+        <v>17100.640108396143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D54D5EE3-8D97-4BF8-8A0C-B511E7D89C8E}">
+  <dimension ref="A4:K26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>1.052E-3</v>
+      </c>
+      <c r="K6">
+        <f>E6/F6</f>
+        <v>7604.5627376425855</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <v>152</v>
+      </c>
+      <c r="F7">
+        <v>9.1339000000000004E-2</v>
+      </c>
+      <c r="K7">
+        <f>E7/F7</f>
+        <v>1664.1303276803994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>746</v>
+      </c>
+      <c r="C8">
+        <v>746</v>
+      </c>
+      <c r="E8">
+        <v>10944</v>
+      </c>
+      <c r="F8">
+        <v>13.968</v>
+      </c>
+      <c r="G8">
+        <v>14</v>
+      </c>
+      <c r="K8">
+        <f>E8/F8</f>
+        <v>783.5051546391752</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>746</v>
+      </c>
+      <c r="C13">
+        <v>283</v>
+      </c>
+      <c r="D13">
+        <v>1411</v>
+      </c>
+      <c r="E13">
+        <v>10944</v>
+      </c>
+      <c r="F13">
+        <v>2.423</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>1.4890000000000001</v>
+      </c>
+      <c r="K13">
+        <f>E13/F13</f>
+        <v>4516.7148163433758</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>567207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>72</v>
+      </c>
+      <c r="C19">
+        <v>71</v>
+      </c>
+      <c r="E19">
+        <v>624</v>
+      </c>
+      <c r="F19">
+        <v>1.52698</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>72</v>
+      </c>
+      <c r="C24">
+        <v>71</v>
+      </c>
+      <c r="D24">
+        <v>109</v>
+      </c>
+      <c r="E24">
+        <v>624</v>
+      </c>
+      <c r="F24">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="K24">
+        <f>E24/F24</f>
+        <v>1124.3243243243242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>12151</v>
+      </c>
+      <c r="C25">
+        <v>12147</v>
+      </c>
+      <c r="D25">
+        <v>23746</v>
+      </c>
+      <c r="E25">
+        <v>233808</v>
+      </c>
+      <c r="F25">
+        <v>201.76</v>
+      </c>
+      <c r="G25">
+        <v>202</v>
+      </c>
+      <c r="H25">
+        <v>66.697999999999993</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>53146457</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>